<commit_message>
new results for fix opt retrofit
</commit_message>
<xml_diff>
--- a/Results/Fixed_optRetrofit_randTornado/15M-1.xlsx
+++ b/Results/Fixed_optRetrofit_randTornado/15M-1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\Results\Fixed_optRetrofit_randTornado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5B15AC8A-B8ED-4B87-A617-E094B1D24299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{035783BE-31A8-49DD-A583-D35A9EFA8B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
-    <sheet name="15M-1" sheetId="1" r:id="rId1"/>
+    <sheet name="2022-10-22_19-23-08_Joplin_100C" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -667,7 +667,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B796D0E-9EE9-2A80-BA93-ECF0F4E472AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37EA7D8C-6AC4-87AA-9D7C-0D9357051F15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -996,7 +996,7 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>10009</v>
+        <v>5030</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1028,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>10053</v>
+        <v>5031</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1044,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>9.18</v>
+        <v>15.85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1060,7 +1060,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>9.01</v>
+        <v>15.61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1068,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1076,7 +1076,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.57999999999999996</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1084,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1092,7 +1092,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1100,10 +1100,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>-94.513000000000005</v>
+        <v>-94.537000000000006</v>
       </c>
       <c r="C12">
-        <v>37.045999999999999</v>
+        <v>37.072000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1111,10 +1111,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-94.49</v>
+        <v>-94.506</v>
       </c>
       <c r="C13">
-        <v>37.116</v>
+        <v>37.140999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,13 +1514,13 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>587</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1572,13 +1572,13 @@
         <v>318522</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>567</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -1659,13 +1659,13 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>443</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -1717,13 +1717,13 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>706</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -1746,13 +1746,13 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -1862,13 +1862,13 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>730</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -1891,13 +1891,13 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>535</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -1949,13 +1949,13 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>702</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -2065,13 +2065,13 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H47">
         <v>0</v>
       </c>
       <c r="I47">
-        <v>274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2181,13 +2181,13 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51">
-        <v>775</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -2268,13 +2268,13 @@
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -2297,13 +2297,13 @@
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55">
-        <v>627</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -2384,13 +2384,13 @@
         <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
-        <v>322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2442,13 +2442,13 @@
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60">
-        <v>505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -2471,13 +2471,13 @@
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>5549173</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -2500,13 +2500,13 @@
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H62">
         <v>0</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>579</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2529,13 +2529,13 @@
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="I63">
-        <v>546</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2616,13 +2616,13 @@
         <v>628762</v>
       </c>
       <c r="G66" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
       <c r="I66">
-        <v>723</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -2703,13 +2703,13 @@
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
-        <v>831</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -2732,13 +2732,13 @@
         <v>108310</v>
       </c>
       <c r="G70" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H70">
-        <v>3418418</v>
+        <v>0</v>
       </c>
       <c r="I70">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -2761,13 +2761,13 @@
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H71">
         <v>0</v>
       </c>
       <c r="I71">
-        <v>140</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -2790,13 +2790,13 @@
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H72">
         <v>0</v>
       </c>
       <c r="I72">
-        <v>399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -2819,13 +2819,13 @@
         <v>1037663</v>
       </c>
       <c r="G73" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="I73">
-        <v>996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -2935,13 +2935,13 @@
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H77">
         <v>0</v>
       </c>
       <c r="I77">
-        <v>648</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -2993,13 +2993,13 @@
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
       <c r="I79">
-        <v>789</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -3051,13 +3051,13 @@
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H81">
         <v>0</v>
       </c>
       <c r="I81">
-        <v>413</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -3196,13 +3196,13 @@
         <v>0</v>
       </c>
       <c r="G86" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H86">
         <v>0</v>
       </c>
       <c r="I86">
-        <v>801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -3254,13 +3254,13 @@
         <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H88">
         <v>0</v>
       </c>
       <c r="I88">
-        <v>636</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>